<commit_message>
Up to date with run 22
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_ELC_DKprices.xlsx
+++ b/SubRES_TMPL/SubRes_ELC_DKprices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\KModel_04\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D7CBDE-F3F9-4BA7-8E44-9BF7FAE716A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB914F4-87A9-4307-B28D-4CA5EBA7F311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -881,7 +881,7 @@
   <dimension ref="B1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>